<commit_message>
Trying to commit again with large files not in commit log
</commit_message>
<xml_diff>
--- a/mentors/julianne/data/Prompts_Utterances.xlsx
+++ b/mentors/julianne/data/Prompts_Utterances.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
   <si>
     <t xml:space="preserve">Situation</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t xml:space="preserve">Good night.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_OFF TOPIC_</t>
   </si>
   <si>
     <t xml:space="preserve">I may have said this before.</t>
@@ -271,7 +268,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -597,15 +594,15 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -640,7 +637,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -675,7 +672,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -710,7 +707,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -745,7 +742,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -780,7 +777,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -815,7 +812,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -850,7 +847,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -885,7 +882,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -920,7 +917,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -955,7 +952,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -990,7 +987,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1019,7 +1016,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>4</v>
@@ -2659,10 +2656,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>9</v>
@@ -2670,46 +2667,46 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="C4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gives julianne an OFFTOPIC answer
</commit_message>
<xml_diff>
--- a/mentors/julianne/data/Prompts_Utterances.xlsx
+++ b/mentors/julianne/data/Prompts_Utterances.xlsx
@@ -1,19 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirschner/projects/MentorPAL/mentors/julianne/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="6440" yWindow="1740" windowWidth="31960" windowHeight="14140" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="official" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="stashed" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="in progress" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="official" sheetId="1" r:id="rId1"/>
+    <sheet name="stashed" sheetId="2" r:id="rId2"/>
+    <sheet name="in progress" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -22,146 +32,128 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
-  <si>
-    <t xml:space="preserve">Situation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mentor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utterance/Prompt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_INTRO_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">juliannenordhagen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi my name's Julie Nordhagen, I'm in the United States Navy and I'm currently a student naval aviator so that means that I have commissioned into the Navy and I am starting to learn how to fly planes and will then become a full trained pilot for the Navy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_FEEDBACK_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes sir.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Excuse me?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How are you?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good morning.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good afternoon.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good evening.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good night.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I may have said this before.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maybe.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perhaps.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Of course.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Always.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Never.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Often.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I do.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I don't</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I have no idea.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I do not think so</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_IDLE_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_PROMPT_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dandavis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_REPEAT_, _OFF_TOPIC_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can you ask me something else?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you have any more questions for me?</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
+  <si>
+    <t>Situation</t>
+  </si>
+  <si>
+    <t>Mentor</t>
+  </si>
+  <si>
+    <t>Utterance/Prompt</t>
+  </si>
+  <si>
+    <t>_INTRO_</t>
+  </si>
+  <si>
+    <t>juliannenordhagen</t>
+  </si>
+  <si>
+    <t>Hi my name's Julie Nordhagen, I'm in the United States Navy and I'm currently a student naval aviator so that means that I have commissioned into the Navy and I am starting to learn how to fly planes and will then become a full trained pilot for the Navy.</t>
+  </si>
+  <si>
+    <t>_FEEDBACK_</t>
+  </si>
+  <si>
+    <t>Yes sir.</t>
+  </si>
+  <si>
+    <t>Excuse me?</t>
+  </si>
+  <si>
+    <t>How are you?</t>
+  </si>
+  <si>
+    <t>Good morning.</t>
+  </si>
+  <si>
+    <t>Good afternoon.</t>
+  </si>
+  <si>
+    <t>Good evening.</t>
+  </si>
+  <si>
+    <t>Good night.</t>
+  </si>
+  <si>
+    <t>I may have said this before.</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Maybe.</t>
+  </si>
+  <si>
+    <t>Perhaps.</t>
+  </si>
+  <si>
+    <t>Of course.</t>
+  </si>
+  <si>
+    <t>Always.</t>
+  </si>
+  <si>
+    <t>Never.</t>
+  </si>
+  <si>
+    <t>Often.</t>
+  </si>
+  <si>
+    <t>I do.</t>
+  </si>
+  <si>
+    <t>I don't</t>
+  </si>
+  <si>
+    <t>I have no idea.</t>
+  </si>
+  <si>
+    <t>I do not think so</t>
+  </si>
+  <si>
+    <t>_IDLE_</t>
+  </si>
+  <si>
+    <t>_PROMPT_</t>
+  </si>
+  <si>
+    <t>dandavis</t>
+  </si>
+  <si>
+    <t>_REPEAT_, _OFF_TOPIC_</t>
+  </si>
+  <si>
+    <t>Can you ask me something else?</t>
+  </si>
+  <si>
+    <t>Do you have any more questions for me?</t>
   </si>
   <si>
     <t xml:space="preserve">Would you mind if I asked you a question? Why are you interested in the Navy? </t>
   </si>
   <si>
-    <t xml:space="preserve">Anything else?</t>
+    <t>Anything else?</t>
+  </si>
+  <si>
+    <t>_OFF_TOPIC_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="PT Sans"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -180,7 +172,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -188,98 +180,326 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AA76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="68.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="68.83203125" customWidth="1"/>
+    <col min="4" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -314,7 +534,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:27" ht="39" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -349,7 +569,7 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -384,9 +604,9 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -419,7 +639,7 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -454,7 +674,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -489,7 +709,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -524,7 +744,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -559,7 +779,7 @@
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -594,7 +814,7 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -629,7 +849,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -664,7 +884,7 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -699,7 +919,7 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -734,7 +954,7 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -769,7 +989,7 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -804,7 +1024,7 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -839,7 +1059,7 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -874,7 +1094,7 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -909,7 +1129,7 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -944,7 +1164,7 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -979,7 +1199,7 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1014,7 +1234,7 @@
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -1047,7 +1267,7 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="4"/>
@@ -1076,7 +1296,7 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="4"/>
@@ -1105,7 +1325,7 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="4"/>
@@ -1134,7 +1354,7 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1163,7 +1383,7 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1192,7 +1412,7 @@
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1221,7 +1441,7 @@
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1250,7 +1470,7 @@
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1279,7 +1499,7 @@
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1308,7 +1528,7 @@
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1337,7 +1557,7 @@
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1366,7 +1586,7 @@
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1395,7 +1615,7 @@
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1424,7 +1644,7 @@
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1453,7 +1673,7 @@
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1482,7 +1702,7 @@
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1511,7 +1731,7 @@
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1540,7 +1760,7 @@
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1569,7 +1789,7 @@
       <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1598,7 +1818,7 @@
       <c r="Z41" s="1"/>
       <c r="AA41" s="1"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1627,7 +1847,7 @@
       <c r="Z42" s="1"/>
       <c r="AA42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1656,7 +1876,7 @@
       <c r="Z43" s="1"/>
       <c r="AA43" s="1"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1685,7 +1905,7 @@
       <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1714,7 +1934,7 @@
       <c r="Z45" s="1"/>
       <c r="AA45" s="1"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1743,7 +1963,7 @@
       <c r="Z46" s="1"/>
       <c r="AA46" s="1"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1772,7 +1992,7 @@
       <c r="Z47" s="1"/>
       <c r="AA47" s="1"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1801,7 +2021,7 @@
       <c r="Z48" s="1"/>
       <c r="AA48" s="1"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1830,7 +2050,7 @@
       <c r="Z49" s="1"/>
       <c r="AA49" s="1"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1859,7 +2079,7 @@
       <c r="Z50" s="1"/>
       <c r="AA50" s="1"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1888,7 +2108,7 @@
       <c r="Z51" s="1"/>
       <c r="AA51" s="1"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1917,7 +2137,7 @@
       <c r="Z52" s="1"/>
       <c r="AA52" s="1"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1946,7 +2166,7 @@
       <c r="Z53" s="1"/>
       <c r="AA53" s="1"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1975,7 +2195,7 @@
       <c r="Z54" s="1"/>
       <c r="AA54" s="1"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2004,7 +2224,7 @@
       <c r="Z55" s="1"/>
       <c r="AA55" s="1"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2033,7 +2253,7 @@
       <c r="Z56" s="1"/>
       <c r="AA56" s="1"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2062,7 +2282,7 @@
       <c r="Z57" s="1"/>
       <c r="AA57" s="1"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2091,7 +2311,7 @@
       <c r="Z58" s="1"/>
       <c r="AA58" s="1"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2120,7 +2340,7 @@
       <c r="Z59" s="1"/>
       <c r="AA59" s="1"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2149,7 +2369,7 @@
       <c r="Z60" s="1"/>
       <c r="AA60" s="1"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2178,7 +2398,7 @@
       <c r="Z61" s="1"/>
       <c r="AA61" s="1"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2207,7 +2427,7 @@
       <c r="Z62" s="1"/>
       <c r="AA62" s="1"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2236,7 +2456,7 @@
       <c r="Z63" s="1"/>
       <c r="AA63" s="1"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2265,7 +2485,7 @@
       <c r="Z64" s="1"/>
       <c r="AA64" s="1"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="4"/>
@@ -2294,7 +2514,7 @@
       <c r="Z65" s="1"/>
       <c r="AA65" s="1"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2323,7 +2543,7 @@
       <c r="Z66" s="1"/>
       <c r="AA66" s="1"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2352,7 +2572,7 @@
       <c r="Z67" s="1"/>
       <c r="AA67" s="1"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2381,7 +2601,7 @@
       <c r="Z68" s="1"/>
       <c r="AA68" s="1"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2410,7 +2630,7 @@
       <c r="Z69" s="1"/>
       <c r="AA69" s="1"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2439,7 +2659,7 @@
       <c r="Z70" s="1"/>
       <c r="AA70" s="1"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2468,7 +2688,7 @@
       <c r="Z71" s="1"/>
       <c r="AA71" s="1"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2497,7 +2717,7 @@
       <c r="Z72" s="1"/>
       <c r="AA72" s="1"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2526,7 +2746,7 @@
       <c r="Z73" s="1"/>
       <c r="AA73" s="1"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2555,7 +2775,7 @@
       <c r="Z74" s="1"/>
       <c r="AA74" s="1"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2584,7 +2804,7 @@
       <c r="Z75" s="1"/>
       <c r="AA75" s="1"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="5"/>
@@ -2614,36 +2834,27 @@
       <c r="AA76" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="4" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2654,7 +2865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
@@ -2665,7 +2876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
@@ -2676,7 +2887,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
@@ -2687,7 +2898,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>27</v>
       </c>
@@ -2698,7 +2909,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
@@ -2710,35 +2921,25 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
+    <col min="1" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="44.5" customWidth="1"/>
+    <col min="4" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2750,12 +2951,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix classifier regression (#46)
* remove root .elasticbeanstalk (not used)

* move classifer out of services and simplfify builds to not use explicit tags locally

* in project root, make sure classifier (base) docker image is rebuild for `make docker-build-services`

* cleanup LSTMClassifier to not print outdated warnings about how to download missing models

* reduce number of default epochs for training (now known to be useless) topic model

* added a new trained lstm_v1 checkpoint. Somehow last checkpoint had corrupt/non-functioning weights for carlos and julianne

* remove WATSON from web app

* optimize docker build for web app/gatsby

* when saving a new checkpoint for lstm_v1, needs to save a marker for the word-2-vec model with each mentor

* gives julianne an OFFTOPIC answer
</commit_message>
<xml_diff>
--- a/mentors/julianne/data/Prompts_Utterances.xlsx
+++ b/mentors/julianne/data/Prompts_Utterances.xlsx
@@ -1,19 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirschner/projects/MentorPAL/mentors/julianne/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="6440" yWindow="1740" windowWidth="31960" windowHeight="14140" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="official" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="stashed" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="in progress" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="official" sheetId="1" r:id="rId1"/>
+    <sheet name="stashed" sheetId="2" r:id="rId2"/>
+    <sheet name="in progress" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -22,146 +32,128 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
-  <si>
-    <t xml:space="preserve">Situation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mentor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utterance/Prompt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_INTRO_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">juliannenordhagen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi my name's Julie Nordhagen, I'm in the United States Navy and I'm currently a student naval aviator so that means that I have commissioned into the Navy and I am starting to learn how to fly planes and will then become a full trained pilot for the Navy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_FEEDBACK_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes sir.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Excuse me?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How are you?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good morning.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good afternoon.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good evening.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good night.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I may have said this before.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maybe.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perhaps.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Of course.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Always.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Never.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Often.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I do.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I don't</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I have no idea.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I do not think so</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_IDLE_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_PROMPT_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dandavis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_REPEAT_, _OFF_TOPIC_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can you ask me something else?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you have any more questions for me?</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
+  <si>
+    <t>Situation</t>
+  </si>
+  <si>
+    <t>Mentor</t>
+  </si>
+  <si>
+    <t>Utterance/Prompt</t>
+  </si>
+  <si>
+    <t>_INTRO_</t>
+  </si>
+  <si>
+    <t>juliannenordhagen</t>
+  </si>
+  <si>
+    <t>Hi my name's Julie Nordhagen, I'm in the United States Navy and I'm currently a student naval aviator so that means that I have commissioned into the Navy and I am starting to learn how to fly planes and will then become a full trained pilot for the Navy.</t>
+  </si>
+  <si>
+    <t>_FEEDBACK_</t>
+  </si>
+  <si>
+    <t>Yes sir.</t>
+  </si>
+  <si>
+    <t>Excuse me?</t>
+  </si>
+  <si>
+    <t>How are you?</t>
+  </si>
+  <si>
+    <t>Good morning.</t>
+  </si>
+  <si>
+    <t>Good afternoon.</t>
+  </si>
+  <si>
+    <t>Good evening.</t>
+  </si>
+  <si>
+    <t>Good night.</t>
+  </si>
+  <si>
+    <t>I may have said this before.</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Maybe.</t>
+  </si>
+  <si>
+    <t>Perhaps.</t>
+  </si>
+  <si>
+    <t>Of course.</t>
+  </si>
+  <si>
+    <t>Always.</t>
+  </si>
+  <si>
+    <t>Never.</t>
+  </si>
+  <si>
+    <t>Often.</t>
+  </si>
+  <si>
+    <t>I do.</t>
+  </si>
+  <si>
+    <t>I don't</t>
+  </si>
+  <si>
+    <t>I have no idea.</t>
+  </si>
+  <si>
+    <t>I do not think so</t>
+  </si>
+  <si>
+    <t>_IDLE_</t>
+  </si>
+  <si>
+    <t>_PROMPT_</t>
+  </si>
+  <si>
+    <t>dandavis</t>
+  </si>
+  <si>
+    <t>_REPEAT_, _OFF_TOPIC_</t>
+  </si>
+  <si>
+    <t>Can you ask me something else?</t>
+  </si>
+  <si>
+    <t>Do you have any more questions for me?</t>
   </si>
   <si>
     <t xml:space="preserve">Would you mind if I asked you a question? Why are you interested in the Navy? </t>
   </si>
   <si>
-    <t xml:space="preserve">Anything else?</t>
+    <t>Anything else?</t>
+  </si>
+  <si>
+    <t>_OFF_TOPIC_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="PT Sans"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -180,7 +172,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -188,98 +180,326 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AA76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="68.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="68.83203125" customWidth="1"/>
+    <col min="4" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -314,7 +534,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:27" ht="39" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -349,7 +569,7 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -384,9 +604,9 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -419,7 +639,7 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -454,7 +674,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -489,7 +709,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -524,7 +744,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -559,7 +779,7 @@
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -594,7 +814,7 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -629,7 +849,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -664,7 +884,7 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -699,7 +919,7 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -734,7 +954,7 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -769,7 +989,7 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -804,7 +1024,7 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -839,7 +1059,7 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -874,7 +1094,7 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -909,7 +1129,7 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -944,7 +1164,7 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -979,7 +1199,7 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1014,7 +1234,7 @@
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -1047,7 +1267,7 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="4"/>
@@ -1076,7 +1296,7 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="4"/>
@@ -1105,7 +1325,7 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="4"/>
@@ -1134,7 +1354,7 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1163,7 +1383,7 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1192,7 +1412,7 @@
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1221,7 +1441,7 @@
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1250,7 +1470,7 @@
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1279,7 +1499,7 @@
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1308,7 +1528,7 @@
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1337,7 +1557,7 @@
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1366,7 +1586,7 @@
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1395,7 +1615,7 @@
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1424,7 +1644,7 @@
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1453,7 +1673,7 @@
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1482,7 +1702,7 @@
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1511,7 +1731,7 @@
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1540,7 +1760,7 @@
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1569,7 +1789,7 @@
       <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1598,7 +1818,7 @@
       <c r="Z41" s="1"/>
       <c r="AA41" s="1"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1627,7 +1847,7 @@
       <c r="Z42" s="1"/>
       <c r="AA42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1656,7 +1876,7 @@
       <c r="Z43" s="1"/>
       <c r="AA43" s="1"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1685,7 +1905,7 @@
       <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1714,7 +1934,7 @@
       <c r="Z45" s="1"/>
       <c r="AA45" s="1"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1743,7 +1963,7 @@
       <c r="Z46" s="1"/>
       <c r="AA46" s="1"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1772,7 +1992,7 @@
       <c r="Z47" s="1"/>
       <c r="AA47" s="1"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1801,7 +2021,7 @@
       <c r="Z48" s="1"/>
       <c r="AA48" s="1"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1830,7 +2050,7 @@
       <c r="Z49" s="1"/>
       <c r="AA49" s="1"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1859,7 +2079,7 @@
       <c r="Z50" s="1"/>
       <c r="AA50" s="1"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1888,7 +2108,7 @@
       <c r="Z51" s="1"/>
       <c r="AA51" s="1"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1917,7 +2137,7 @@
       <c r="Z52" s="1"/>
       <c r="AA52" s="1"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1946,7 +2166,7 @@
       <c r="Z53" s="1"/>
       <c r="AA53" s="1"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1975,7 +2195,7 @@
       <c r="Z54" s="1"/>
       <c r="AA54" s="1"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2004,7 +2224,7 @@
       <c r="Z55" s="1"/>
       <c r="AA55" s="1"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2033,7 +2253,7 @@
       <c r="Z56" s="1"/>
       <c r="AA56" s="1"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2062,7 +2282,7 @@
       <c r="Z57" s="1"/>
       <c r="AA57" s="1"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2091,7 +2311,7 @@
       <c r="Z58" s="1"/>
       <c r="AA58" s="1"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2120,7 +2340,7 @@
       <c r="Z59" s="1"/>
       <c r="AA59" s="1"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2149,7 +2369,7 @@
       <c r="Z60" s="1"/>
       <c r="AA60" s="1"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2178,7 +2398,7 @@
       <c r="Z61" s="1"/>
       <c r="AA61" s="1"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2207,7 +2427,7 @@
       <c r="Z62" s="1"/>
       <c r="AA62" s="1"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2236,7 +2456,7 @@
       <c r="Z63" s="1"/>
       <c r="AA63" s="1"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2265,7 +2485,7 @@
       <c r="Z64" s="1"/>
       <c r="AA64" s="1"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="4"/>
@@ -2294,7 +2514,7 @@
       <c r="Z65" s="1"/>
       <c r="AA65" s="1"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2323,7 +2543,7 @@
       <c r="Z66" s="1"/>
       <c r="AA66" s="1"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2352,7 +2572,7 @@
       <c r="Z67" s="1"/>
       <c r="AA67" s="1"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2381,7 +2601,7 @@
       <c r="Z68" s="1"/>
       <c r="AA68" s="1"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2410,7 +2630,7 @@
       <c r="Z69" s="1"/>
       <c r="AA69" s="1"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2439,7 +2659,7 @@
       <c r="Z70" s="1"/>
       <c r="AA70" s="1"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2468,7 +2688,7 @@
       <c r="Z71" s="1"/>
       <c r="AA71" s="1"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2497,7 +2717,7 @@
       <c r="Z72" s="1"/>
       <c r="AA72" s="1"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2526,7 +2746,7 @@
       <c r="Z73" s="1"/>
       <c r="AA73" s="1"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2555,7 +2775,7 @@
       <c r="Z74" s="1"/>
       <c r="AA74" s="1"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2584,7 +2804,7 @@
       <c r="Z75" s="1"/>
       <c r="AA75" s="1"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="5"/>
@@ -2614,36 +2834,27 @@
       <c r="AA76" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="4" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2654,7 +2865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
@@ -2665,7 +2876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
@@ -2676,7 +2887,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
@@ -2687,7 +2898,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>27</v>
       </c>
@@ -2698,7 +2909,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
@@ -2710,35 +2921,25 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
+    <col min="1" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="44.5" customWidth="1"/>
+    <col min="4" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2750,12 +2951,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>